<commit_message>
update ward 1 yojana haru nearly complete
</commit_message>
<xml_diff>
--- a/ward 1 yojana haru.xlsx
+++ b/ward 1 yojana haru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2082_2083\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C412B4D-03B2-4FEB-935B-4BC50E85F880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF13A7E-7AEF-4762-929D-E4C8C864F21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="124">
   <si>
     <t>qm= ;+=</t>
   </si>
@@ -175,6 +175,237 @@
   </si>
   <si>
     <t>z+v/fk'/ ! leqsf laleGg ;fd'bflos ejgx? -9sfn ;fd'bflos ejg, nfdf 6f]n ;fd'bflos ejg, x}a'ªu6f]n u'l7 ejg, uf}?ª 6n ;fd'bflos ejg_</t>
+  </si>
+  <si>
+    <t>;8s k'n</t>
+  </si>
+  <si>
+    <t>ltg3/] af6f] :t/f]GgtL</t>
+  </si>
+  <si>
+    <t>nfs'l/af]6 s'08]Zj/ ;8s</t>
+  </si>
+  <si>
+    <t>@%)))))</t>
+  </si>
+  <si>
+    <t>z+v/fk'/ ! leqsf laleGg ;8sx? -cf]v/af]6 g]kfn6f]n ;8s, lgKnfl;d lt;'{n] ;8s, 3'lDt vgfn 6f]n ;8s, lhDNof6f/ cDkm] ;8s, eb]|cfn emfFlqm 9'ªuf ;8s, lahf}/] ;8s, ltg3/] ;8s_</t>
+  </si>
+  <si>
+    <t>!*)))))</t>
+  </si>
+  <si>
+    <t>l;uf/] kf}jf 9'ufgf a]lz ;8s</t>
+  </si>
+  <si>
+    <t>hut] rf}ls eG‰ofª ;8s</t>
+  </si>
+  <si>
+    <t>a+ufln 8f8f lhNs]6f]n ;8s</t>
+  </si>
+  <si>
+    <t>;'s'kfgL ljhf}}/] j:tL tyf s[lif ;8s</t>
+  </si>
+  <si>
+    <t>5fk 9sfn6f]n a/faf]6 ;8s</t>
+  </si>
+  <si>
+    <t>nfdflj;f}gf d]n 8fF8f ;8s</t>
+  </si>
+  <si>
+    <t>nfFs'/Ljf]6 b]jL ;'df/f ;8s</t>
+  </si>
+  <si>
+    <t>z+v/fk'/ ! leqsf laleGg l;rfO{ -;'s'kfgL l;/fg l;rfO{, lhDn]6f/ l;rfO{, nK;] l;rfO{, cf]8f/] l;rfO{, l/dfn 38]l/ l;rfO{, u0f]z] l;+rfO{_</t>
+  </si>
+  <si>
+    <t>l;+rfO{</t>
+  </si>
+  <si>
+    <t>b]jL:yfg vfgL8fF8f l;+rfO{</t>
+  </si>
+  <si>
+    <t>x}j'ª 8fF8f3/]6f]n klx/f] ;+/If0f</t>
+  </si>
+  <si>
+    <t>jftfj/0f tyf ljkb\ Joj:yfkg</t>
+  </si>
+  <si>
+    <t>j8f g+= ! leqsf laljw ;8s dd{t</t>
+  </si>
+  <si>
+    <t>!!)%)))</t>
+  </si>
+  <si>
+    <t>6]G8/df uPsf qmdfut of]hgf</t>
+  </si>
+  <si>
+    <t>!)</t>
+  </si>
+  <si>
+    <t>!!</t>
+  </si>
+  <si>
+    <t>!#</t>
+  </si>
+  <si>
+    <t>"!@</t>
+  </si>
+  <si>
+    <t>!$</t>
+  </si>
+  <si>
+    <t>!%</t>
+  </si>
+  <si>
+    <t>!^</t>
+  </si>
+  <si>
+    <t>!&amp;</t>
+  </si>
+  <si>
+    <t>!*</t>
+  </si>
+  <si>
+    <t>!(</t>
+  </si>
+  <si>
+    <t>@)</t>
+  </si>
+  <si>
+    <t>@!</t>
+  </si>
+  <si>
+    <t>@@</t>
+  </si>
+  <si>
+    <t>@#</t>
+  </si>
+  <si>
+    <t>@$</t>
+  </si>
+  <si>
+    <t>@%</t>
+  </si>
+  <si>
+    <t>@^</t>
+  </si>
+  <si>
+    <t>@&amp;</t>
+  </si>
+  <si>
+    <t>@*</t>
+  </si>
+  <si>
+    <t>@(</t>
+  </si>
+  <si>
+    <t>j8fut of]hgf</t>
+  </si>
+  <si>
+    <t>dfg]u}/f] nfdf6f]n ;8s</t>
+  </si>
+  <si>
+    <t>laljw ;8s ;/;kmfO{</t>
+  </si>
+  <si>
+    <t>*)))))</t>
+  </si>
+  <si>
+    <t>e}kl/ kF'hLut vr{</t>
+  </si>
+  <si>
+    <t>!))))))</t>
+  </si>
+  <si>
+    <t>;+3Lo ;/sf/af6 x:tfGtl/t sfo{qmd</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! 8fF8fyf]s tfdfª a:tL ljsf; sfo{qmd cGtu{t k"jf{wf/ :t/f]Gglt sfo{</t>
+  </si>
+  <si>
+    <t>$))))))</t>
+  </si>
+  <si>
+    <t>#)</t>
+  </si>
+  <si>
+    <t>#!</t>
+  </si>
+  <si>
+    <t>#@</t>
+  </si>
+  <si>
+    <t>##</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! 5fk 9sfn 6f]n emfFs] al:t ;8s :t/f]Gglt sfo{</t>
+  </si>
+  <si>
+    <t>#$</t>
+  </si>
+  <si>
+    <t>#%</t>
+  </si>
+  <si>
+    <t>&amp;))))))</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! Gffªn] ahf/–vqLufpF–kf]v/L vf]nf–z+v/fk'/ ;8s :t/f]Gglt sfo{</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! kfËu|]af; cfn8fF8f ;f]tL xn]b] ;8s :t/f]Gglt sfo{</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! Kff]v/L rf}/ 9'ªØfg g]jf/ 6f]n eHofË ;8s :t/f]Gglt sfo{</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! ah|of]lugL dfO{ dlGb/ kl/;/ ;'wf/ Pj+ /y /fVg] kf6L{ lgdf{0f</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! dgf]x/f zfnLgbL sl/8f]/</t>
+  </si>
+  <si>
+    <t>sf7df8f}F lhNnf z+v/fk'/ gu/kflnsf j8f g+ ! z+v/fk'/ j8f g+ ! sf] sfof{no b]lv k+rkfn] xn]b] r'/]y'Ëf sfe|] hf]8\g] ;8s :t/f]Gglt sfo{</t>
+  </si>
+  <si>
+    <t>#^</t>
+  </si>
+  <si>
+    <t>#&amp;</t>
+  </si>
+  <si>
+    <t>#*</t>
+  </si>
+  <si>
+    <t>#(</t>
+  </si>
+  <si>
+    <t>$)</t>
+  </si>
+  <si>
+    <t>s]/faf/L s'08]Zj/ gofF 6«fs s[lif ;8s, z+v/fk'/ !</t>
+  </si>
+  <si>
+    <t>s[lif pkh ;+sng s]Gb« lgdf{0f – z+v/fk'/–!</t>
+  </si>
+  <si>
+    <t>!%)))))</t>
+  </si>
+  <si>
+    <t>k|b]z ;/sf/af6 x:tfGtl/t sfo{qmd</t>
+  </si>
+  <si>
+    <t>9sfn6f]n vfgL8fF8f s[lif ;8s, z+v/fk'/ !</t>
+  </si>
+  <si>
+    <t>$!</t>
+  </si>
+  <si>
+    <t>$@</t>
+  </si>
+  <si>
+    <t>$#</t>
   </si>
 </sst>
 </file>
@@ -255,12 +486,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -269,23 +497,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H30"/>
+  <dimension ref="B1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,393 +831,925 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="6" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="2:8" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="12" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="2:8" ht="144" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" s="14" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="s">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:8" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:8" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="14" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+      <c r="C21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="2:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="15" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="s">
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="2:8" ht="72" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8" t="s">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="2:8" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
+      <c r="D24" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="30" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="2:8" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="2:8" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="B40" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="2:8" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B44" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B48" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B50" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B51" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B52" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B53" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B54" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+    </row>
+    <row r="55" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B55" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+    </row>
+    <row r="56" spans="2:8" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+    </row>
+    <row r="57" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+    </row>
+    <row r="58" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B58" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+    </row>
+    <row r="59" spans="2:8" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+    </row>
+    <row r="61" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="63" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>